<commit_message>
updated Stand up meeting Templet and added my assigned tasks
Saibabu Devarapalli
</commit_message>
<xml_diff>
--- a/Sprint2/Stand-up Meeting Sprint2.xlsx
+++ b/Sprint2/Stand-up Meeting Sprint2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s546907\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S547049\Documents\GitHub\Sec03Team05Fall22GDP1\Sprint2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{072AA6FE-E9E2-4CA5-A798-2159F90D53F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BFE1A57-12A6-4CCB-B800-04AE0F8CE660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="35">
   <si>
     <t>Monday</t>
   </si>
@@ -162,6 +162,34 @@
   </si>
   <si>
     <t>3) Come up with layouts that are best suitable for our project. Team will propose different layout designs we will finalize them</t>
+  </si>
+  <si>
+    <t>1) Freebies for Newbies is a project that assists new international students and will be helpful to their needs. We decide to cut the project budget and enhance the functioning of a task which results in user friendly Application.</t>
+  </si>
+  <si>
+    <t>1) We created a workflow as a team, and we assigned tasks for this week. worked on layout pages, database tools, and software requirements.</t>
+  </si>
+  <si>
+    <t>1) worked on the layout of the pages for sign-up and sign-in.</t>
+  </si>
+  <si>
+    <t>2) As a team, we will assign tasks and choose the database and backend technologies that are best for the project. We'll create a blueprint.</t>
+  </si>
+  <si>
+    <t>2) We'll take the necessary steps to link user-entered data to the database and get a quick response. Additionally, we will work on page layout and gather team updates.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2) will focus on how input data from the UI linked to the database and work on backend coding to transfer data from the database to the UI.
+</t>
+  </si>
+  <si>
+    <t>3) It could be challenging to assign tasks and time complexity.</t>
+  </si>
+  <si>
+    <t>3) Conflicts might arise while connecting user-provided data to a database and receiving responses from the database to the front end.</t>
+  </si>
+  <si>
+    <t>3) We will learn more about Android Studio and the Firebase database as we gain a better understanding of its basics.</t>
   </si>
 </sst>
 </file>
@@ -222,7 +250,7 @@
       <name val="Times New Roman"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -247,8 +275,14 @@
         <bgColor rgb="FFF2F2F2"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -312,11 +346,71 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -331,6 +425,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -350,8 +447,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -635,8 +741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -648,52 +754,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
@@ -715,45 +821,45 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="46.5" x14ac:dyDescent="0.3">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="D8" s="8" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="31" x14ac:dyDescent="0.3">
-      <c r="A9" s="11"/>
-      <c r="B9" s="15" t="s">
+      <c r="A9" s="12"/>
+      <c r="B9" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="15" t="s">
+      <c r="D9" s="8" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="62" x14ac:dyDescent="0.3">
-      <c r="A10" s="11"/>
-      <c r="B10" s="15" t="s">
+      <c r="A10" s="12"/>
+      <c r="B10" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="D10" s="8" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="11" t="s">
         <v>13</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -767,7 +873,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="A12" s="10"/>
+      <c r="A12" s="11"/>
       <c r="B12" s="3" t="s">
         <v>5</v>
       </c>
@@ -778,8 +884,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="A13" s="10"/>
+    <row r="13" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="11"/>
       <c r="B13" s="3" t="s">
         <v>6</v>
       </c>
@@ -790,46 +896,46 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="A14" s="11" t="s">
+    <row r="14" spans="1:6" ht="109" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="A15" s="11"/>
-      <c r="B15" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="A16" s="11"/>
-      <c r="B16" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>6</v>
+      <c r="B14" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="78" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="12"/>
+      <c r="B15" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="62.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="12"/>
+      <c r="B16" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="11" t="s">
         <v>15</v>
       </c>
       <c r="B17" s="3" t="s">
@@ -843,7 +949,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="A18" s="10"/>
+      <c r="A18" s="11"/>
       <c r="B18" s="3" t="s">
         <v>5</v>
       </c>
@@ -855,7 +961,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="A19" s="10"/>
+      <c r="A19" s="11"/>
       <c r="B19" s="3" t="s">
         <v>6</v>
       </c>
@@ -867,7 +973,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="A20" s="11" t="s">
+      <c r="A20" s="12" t="s">
         <v>16</v>
       </c>
       <c r="B20" s="5" t="s">
@@ -881,7 +987,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="A21" s="11"/>
+      <c r="A21" s="12"/>
       <c r="B21" s="5" t="s">
         <v>5</v>
       </c>
@@ -893,7 +999,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="A22" s="11"/>
+      <c r="A22" s="12"/>
       <c r="B22" s="5" t="s">
         <v>6</v>
       </c>
@@ -911,18 +1017,18 @@
       <c r="B25" s="6"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="8" t="s">
+      <c r="A26" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B26" s="9"/>
+      <c r="B26" s="10"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="9"/>
-      <c r="B27" s="9"/>
+      <c r="A27" s="10"/>
+      <c r="B27" s="10"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="9"/>
-      <c r="B28" s="9"/>
+      <c r="A28" s="10"/>
+      <c r="B28" s="10"/>
     </row>
     <row r="32" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -941,7 +1047,7 @@
     <mergeCell ref="A4:F4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Updated Stand-up meeting Template added my Work
Harish Chowdary Bala
</commit_message>
<xml_diff>
--- a/Sprint2/Stand-up Meeting Sprint2.xlsx
+++ b/Sprint2/Stand-up Meeting Sprint2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S547049\Documents\GitHub\Sec03Team05Fall22GDP1\Sprint2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S547076\Desktop\Sec03Team05Fall22GDP1\Sprint2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BFE1A57-12A6-4CCB-B800-04AE0F8CE660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B4B2DD0-D2E8-436E-83D4-FBD38DC46C90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="44">
   <si>
     <t>Monday</t>
   </si>
@@ -190,6 +190,33 @@
   </si>
   <si>
     <t>3) We will learn more about Android Studio and the Firebase database as we gain a better understanding of its basics.</t>
+  </si>
+  <si>
+    <t>Present I don't accomplish anything just discuss about project with team members.</t>
+  </si>
+  <si>
+    <t>.I learn about the firebase database it helps me to do design these project</t>
+  </si>
+  <si>
+    <t>I learn about MongoDB and Firebase Databse</t>
+  </si>
+  <si>
+    <t>Today we discuss about the data of everyone is collected and what type of technologies are used in these design.</t>
+  </si>
+  <si>
+    <t>Yesterday we discuss about the design of these project and we are working on these assigned work.</t>
+  </si>
+  <si>
+    <t>2)I will continue the which work assigned by team discussion.</t>
+  </si>
+  <si>
+    <t>We are confusing about team roles and work structure.</t>
+  </si>
+  <si>
+    <t>I don't know about andriod studio, So I am working on that.</t>
+  </si>
+  <si>
+    <t>I have no experience and I learning it will take some time.</t>
   </si>
 </sst>
 </file>
@@ -410,7 +437,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -420,14 +447,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -446,18 +482,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -741,8 +765,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -754,52 +778,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
@@ -821,45 +845,45 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="46.5" x14ac:dyDescent="0.3">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="7" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="31" x14ac:dyDescent="0.3">
-      <c r="A9" s="12"/>
-      <c r="B9" s="8" t="s">
+      <c r="A9" s="15"/>
+      <c r="B9" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="7" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="62" x14ac:dyDescent="0.3">
-      <c r="A10" s="12"/>
-      <c r="B10" s="8" t="s">
+      <c r="A10" s="15"/>
+      <c r="B10" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="7" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="14" t="s">
         <v>13</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -873,7 +897,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="A12" s="11"/>
+      <c r="A12" s="14"/>
       <c r="B12" s="3" t="s">
         <v>5</v>
       </c>
@@ -885,7 +909,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="11"/>
+      <c r="A13" s="14"/>
       <c r="B13" s="3" t="s">
         <v>6</v>
       </c>
@@ -897,45 +921,45 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="109" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="12" t="s">
+      <c r="A14" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="17" t="s">
+      <c r="C14" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="17" t="s">
+      <c r="D14" s="9" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="78" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="12"/>
-      <c r="B15" s="18" t="s">
+      <c r="A15" s="15"/>
+      <c r="B15" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="19" t="s">
+      <c r="C15" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="19" t="s">
+      <c r="D15" s="11" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="62.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="12"/>
-      <c r="B16" s="18" t="s">
+      <c r="A16" s="15"/>
+      <c r="B16" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="19" t="s">
+      <c r="C16" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D16" s="19" t="s">
+      <c r="D16" s="11" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="14" t="s">
         <v>15</v>
       </c>
       <c r="B17" s="3" t="s">
@@ -949,7 +973,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="A18" s="11"/>
+      <c r="A18" s="14"/>
       <c r="B18" s="3" t="s">
         <v>5</v>
       </c>
@@ -960,8 +984,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="A19" s="11"/>
+    <row r="19" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="14"/>
       <c r="B19" s="3" t="s">
         <v>6</v>
       </c>
@@ -972,63 +996,63 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="A20" s="12" t="s">
+    <row r="20" spans="1:4" ht="47" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="A21" s="12"/>
-      <c r="B21" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="A22" s="12"/>
-      <c r="B22" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>6</v>
+      <c r="B20" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="62.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="15"/>
+      <c r="B21" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="31.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="15"/>
+      <c r="B22" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15" x14ac:dyDescent="0.3">
-      <c r="A25" s="7" t="s">
+      <c r="A25" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B25" s="6"/>
+      <c r="B25" s="5"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="9" t="s">
+      <c r="A26" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B26" s="10"/>
+      <c r="B26" s="13"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="10"/>
-      <c r="B27" s="10"/>
+      <c r="A27" s="13"/>
+      <c r="B27" s="13"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="10"/>
-      <c r="B28" s="10"/>
+      <c r="A28" s="13"/>
+      <c r="B28" s="13"/>
     </row>
     <row r="32" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Updated the daily standup meeting report for adithya
</commit_message>
<xml_diff>
--- a/Sprint2/Stand-up Meeting Sprint2.xlsx
+++ b/Sprint2/Stand-up Meeting Sprint2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S547076\Desktop\Sec03Team05Fall22GDP1\Sprint2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nwmissouri-my.sharepoint.com/personal/s546942_nwmissouri_edu/Documents/Desktop/webapps-repo/Sec03Team05Fall22GDP1/Sprint2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B4B2DD0-D2E8-436E-83D4-FBD38DC46C90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{0B4B2DD0-D2E8-436E-83D4-FBD38DC46C90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9C2F11FC-70A5-4A24-8F30-8B8F39AACC07}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="53">
   <si>
     <t>Monday</t>
   </si>
@@ -217,6 +217,33 @@
   </si>
   <si>
     <t>I have no experience and I learning it will take some time.</t>
+  </si>
+  <si>
+    <t>1) We finalised the project and dicussed how to accomplish goals.</t>
+  </si>
+  <si>
+    <t>1) We discussed about the workflow process and started working on it.</t>
+  </si>
+  <si>
+    <t>1) Wev have completed workflow and one of my team mate submitted workflow structure.</t>
+  </si>
+  <si>
+    <t>2) Discussion about the work breakdown with team mates.</t>
+  </si>
+  <si>
+    <t>2) We discussed about the UI layouts and we need to start working on it.</t>
+  </si>
+  <si>
+    <t>2) We want to start the design phase of the UI for Layouts.</t>
+  </si>
+  <si>
+    <t>3) We need to breakdown work structure.</t>
+  </si>
+  <si>
+    <t>3) Workflow designed we need prior approval of workflow to start the UI design.</t>
+  </si>
+  <si>
+    <t>3) We need to know more about android studio, as we are IOS developer.</t>
   </si>
 </sst>
 </file>
@@ -437,7 +464,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -482,6 +509,18 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -765,8 +804,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11:D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -870,7 +909,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="62" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="62.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="15"/>
       <c r="B10" s="7" t="s">
         <v>23</v>
@@ -882,42 +921,42 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="47" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="15.5" x14ac:dyDescent="0.3">
+      <c r="B11" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="31.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="14"/>
-      <c r="B12" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" s="22" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="47" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="14"/>
-      <c r="B13" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>6</v>
+      <c r="B13" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13" s="22" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="109" thickBot="1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Updated standup meeting.docx sprint2
Manoj Standup meeting sprint2 docx is updated
</commit_message>
<xml_diff>
--- a/Sprint2/Stand-up Meeting Sprint2.xlsx
+++ b/Sprint2/Stand-up Meeting Sprint2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S547076\Desktop\Sec03Team05Fall22GDP1\Sprint2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nwmissouri-my.sharepoint.com/personal/s546981_nwmissouri_edu/Documents/Documents/GitHub/Sec03Team05Fall22GDP1/Sprint2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B4B2DD0-D2E8-436E-83D4-FBD38DC46C90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{0B4B2DD0-D2E8-436E-83D4-FBD38DC46C90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3CD4EDE2-0B68-4748-90D5-052C6871B534}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="53">
   <si>
     <t>Monday</t>
   </si>
@@ -217,6 +217,33 @@
   </si>
   <si>
     <t>I have no experience and I learning it will take some time.</t>
+  </si>
+  <si>
+    <t>2) Assigning team member roles to design work flow diagram</t>
+  </si>
+  <si>
+    <t>1) Pitching project idea, discussed pros and cons of project and assigned team members</t>
+  </si>
+  <si>
+    <t>3)Assigning team member roles is bit difficul</t>
+  </si>
+  <si>
+    <t>1)We as a team discussed about software methodology to follow and discussed about the number of layouts to be placed and software requirements to be installed on every team members device.</t>
+  </si>
+  <si>
+    <t>2)Getting knowledge and designing basic layouts of the application</t>
+  </si>
+  <si>
+    <t>3)Integrating the frontend and database</t>
+  </si>
+  <si>
+    <t>1)Adithya and me shared roles as frontend developers and we are anticipated 5 layout in the application and we discussed with team members about layouts and how layouts has to be designed</t>
+  </si>
+  <si>
+    <t>2)Concentrating on UI and layouts</t>
+  </si>
+  <si>
+    <t>3)Finalizing UI design</t>
   </si>
 </sst>
 </file>
@@ -765,8 +792,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -958,42 +985,42 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15.5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="93" x14ac:dyDescent="0.3">
       <c r="A17" s="14" t="s">
         <v>15</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>4</v>
+        <v>45</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>4</v>
+        <v>47</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="15.5" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="31" x14ac:dyDescent="0.3">
       <c r="A18" s="14"/>
       <c r="B18" s="3" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>5</v>
+        <v>48</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.35">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="31.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="14"/>
       <c r="B19" s="3" t="s">
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>6</v>
+        <v>49</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>6</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="47" thickBot="1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Updated standup meeting docx
Updated manoj standup meeting document
</commit_message>
<xml_diff>
--- a/Sprint2/Stand-up Meeting Sprint2.xlsx
+++ b/Sprint2/Stand-up Meeting Sprint2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nwmissouri-my.sharepoint.com/personal/s546942_nwmissouri_edu/Documents/Desktop/webapps-repo/Sec03Team05Fall22GDP1/Sprint2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nwmissouri-my.sharepoint.com/personal/s546981_nwmissouri_edu/Documents/Documents/GitHub/Sec03Team05Fall22GDP1/Sprint2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{0B4B2DD0-D2E8-436E-83D4-FBD38DC46C90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9C2F11FC-70A5-4A24-8F30-8B8F39AACC07}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{0B4B2DD0-D2E8-436E-83D4-FBD38DC46C90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{533ECA84-86E3-475B-8029-788F9CBCDBDA}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
   <si>
     <t>Monday</t>
   </si>
@@ -40,15 +40,6 @@
   </si>
   <si>
     <t>Daily Stand-up Meeting Report</t>
-  </si>
-  <si>
-    <t>1)</t>
-  </si>
-  <si>
-    <t>2)</t>
-  </si>
-  <si>
-    <t>3)</t>
   </si>
   <si>
     <t>Note:</t>
@@ -244,6 +235,33 @@
   </si>
   <si>
     <t>3) We need to know more about android studio, as we are IOS developer.</t>
+  </si>
+  <si>
+    <t>1) Pitching project idea, discussed pros and cons of project and assigned team members</t>
+  </si>
+  <si>
+    <t>2)Assigning team member roles to design work flow diagram</t>
+  </si>
+  <si>
+    <t>3)Assigning team member roles is bit difficult</t>
+  </si>
+  <si>
+    <t>1)We as a team discussed about software methodology to follow and discussed about the number of layouts to be placed and software requirements to be installed on every team members device.</t>
+  </si>
+  <si>
+    <t>2)Getting knowledge and designing basic layouts of the application</t>
+  </si>
+  <si>
+    <t>3)Integrating the frontend and database</t>
+  </si>
+  <si>
+    <t>1)Adithya and me shared roles as frontend developers and we are anticipated 5 layout in the application and we discussed with team members about layouts and how layouts has to be designed</t>
+  </si>
+  <si>
+    <t>2)Concentrating on UI and layouts</t>
+  </si>
+  <si>
+    <t>3)Finalizing UI design</t>
   </si>
 </sst>
 </file>
@@ -491,6 +509,18 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -509,18 +539,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -804,8 +822,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:D13"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -817,52 +835,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
+      <c r="A2" s="20"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
@@ -884,214 +902,214 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="46.5" x14ac:dyDescent="0.3">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="31" x14ac:dyDescent="0.3">
+      <c r="A9" s="19"/>
+      <c r="B9" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="62.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="19"/>
+      <c r="B10" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="47" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="31.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="18"/>
+      <c r="B12" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="47" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="18"/>
+      <c r="B13" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="109" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="78" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="19"/>
+      <c r="B15" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="62.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="19"/>
+      <c r="B16" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="93" x14ac:dyDescent="0.3">
+      <c r="A17" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="31" x14ac:dyDescent="0.3">
-      <c r="A9" s="15"/>
-      <c r="B9" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="62.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="15"/>
-      <c r="B10" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="47" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="14" t="s">
+      <c r="B17" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="31" x14ac:dyDescent="0.3">
+      <c r="A18" s="18"/>
+      <c r="B18" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="31.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="18"/>
+      <c r="B19" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="47" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="C11" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="D11" s="20" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="31.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="14"/>
-      <c r="B12" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="C12" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="D12" s="22" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="47" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="14"/>
-      <c r="B13" s="21" t="s">
-        <v>50</v>
-      </c>
-      <c r="C13" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="D13" s="22" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="109" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="78" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="15"/>
-      <c r="B15" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="62.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="15"/>
-      <c r="B16" s="10" t="s">
+      <c r="B20" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C20" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D20" s="9" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="A17" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="A18" s="14"/>
-      <c r="B18" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="14"/>
-      <c r="B19" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="47" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="B20" s="8" t="s">
+    <row r="21" spans="1:4" ht="62.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="19"/>
+      <c r="B21" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C21" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="D20" s="9" t="s">
+      <c r="D21" s="11" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="62.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="15"/>
-      <c r="B21" s="10" t="s">
+    <row r="22" spans="1:4" ht="31.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="19"/>
+      <c r="B22" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="C22" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="D21" s="11" t="s">
+      <c r="D22" s="11" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="31.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="15"/>
-      <c r="B22" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="D22" s="11" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B25" s="5"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B26" s="13"/>
+      <c r="A26" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="17"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="13"/>
-      <c r="B27" s="13"/>
+      <c r="A27" s="17"/>
+      <c r="B27" s="17"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="13"/>
-      <c r="B28" s="13"/>
+      <c r="A28" s="17"/>
+      <c r="B28" s="17"/>
     </row>
     <row r="32" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>